<commit_message>
updating GDP and algo
</commit_message>
<xml_diff>
--- a/data/Atlanta_GDP.xlsx
+++ b/data/Atlanta_GDP.xlsx
@@ -1,30 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whelvey\Documents\GitHub\inflation_cr_expansion\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\inflation_cr_expansion\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C4477AB-5EFF-4D8C-B372-8F61950B4C52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7755A2C0-D6DF-484B-9142-11646B0DCF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="114210"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -64,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -412,11 +403,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A12" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -480,7 +471,7 @@
         <v>36892</v>
       </c>
       <c r="B12" s="2">
-        <v>208707.56200000001</v>
+        <v>208125.35500000001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -488,7 +479,7 @@
         <v>37257</v>
       </c>
       <c r="B13" s="2">
-        <v>214456.86</v>
+        <v>214103.45600000001</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -496,7 +487,7 @@
         <v>37622</v>
       </c>
       <c r="B14" s="2">
-        <v>223529.505</v>
+        <v>224545.62899999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -504,7 +495,7 @@
         <v>37987</v>
       </c>
       <c r="B15" s="2">
-        <v>239689.318</v>
+        <v>239911.62400000001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -512,7 +503,7 @@
         <v>38353</v>
       </c>
       <c r="B16" s="2">
-        <v>256152.546</v>
+        <v>257637.92199999999</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -520,7 +511,7 @@
         <v>38718</v>
       </c>
       <c r="B17" s="2">
-        <v>263873.17200000002</v>
+        <v>269153.32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -528,7 +519,7 @@
         <v>39083</v>
       </c>
       <c r="B18" s="2">
-        <v>271150.48300000001</v>
+        <v>277955.08100000001</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -536,7 +527,7 @@
         <v>39448</v>
       </c>
       <c r="B19" s="2">
-        <v>267318.80900000001</v>
+        <v>273531.55099999998</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -544,7 +535,7 @@
         <v>39814</v>
       </c>
       <c r="B20" s="2">
-        <v>261181.36900000001</v>
+        <v>266522.79700000002</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -552,7 +543,7 @@
         <v>40179</v>
       </c>
       <c r="B21" s="2">
-        <v>267528.03200000001</v>
+        <v>272123.15899999999</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -560,7 +551,7 @@
         <v>40544</v>
       </c>
       <c r="B22" s="2">
-        <v>276621.05099999998</v>
+        <v>281302.90500000003</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -568,7 +559,7 @@
         <v>40909</v>
       </c>
       <c r="B23" s="2">
-        <v>287373.83899999998</v>
+        <v>292330.81300000002</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -576,7 +567,7 @@
         <v>41275</v>
       </c>
       <c r="B24" s="2">
-        <v>299317.84100000001</v>
+        <v>305248.97499999998</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -584,7 +575,7 @@
         <v>41640</v>
       </c>
       <c r="B25" s="2">
-        <v>319397.14</v>
+        <v>325002.75699999998</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -592,7 +583,7 @@
         <v>42005</v>
       </c>
       <c r="B26" s="2">
-        <v>341613.08199999999</v>
+        <v>347744.95699999999</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -600,7 +591,7 @@
         <v>42370</v>
       </c>
       <c r="B27" s="2">
-        <v>362885.03499999997</v>
+        <v>369995.897</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -608,7 +599,7 @@
         <v>42736</v>
       </c>
       <c r="B28" s="2">
-        <v>382546.94900000002</v>
+        <v>389471.81300000002</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -616,7 +607,7 @@
         <v>43101</v>
       </c>
       <c r="B29" s="2">
-        <v>406761.58500000002</v>
+        <v>411660.04499999998</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -624,7 +615,15 @@
         <v>43466</v>
       </c>
       <c r="B30" s="2">
-        <v>422189.46100000001</v>
+        <v>438936.81400000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B31" s="2">
+        <v>425443.80699999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>